<commit_message>
Add short lesson on supervised and unsupervised learning
</commit_message>
<xml_diff>
--- a/HTS-Course-Schedule-Final-2018.xlsx
+++ b/HTS-Course-Schedule-Final-2018.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Box Sync/HTS-Course-Development/2018/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cliburn/_teach/HTS2018-notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1241A4D1-35BE-7C44-86DE-F88BB314BD9C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A3E508-09E7-1F49-B28F-8E62A028069B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33520" windowHeight="20540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Bioinformatics 2018" sheetId="3" state="hidden" r:id="rId2"/>
     <sheet name="cleaned" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179016"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -628,9 +628,6 @@
     <t>Comput: Intro to Bioconductor objects (JM, CC)</t>
   </si>
   <si>
-    <t>Compute: Reproducible analysis (CC, KO)</t>
-  </si>
-  <si>
     <t>Tidyverse III (JM, CC)</t>
   </si>
   <si>
@@ -653,6 +650,9 @@
   </si>
   <si>
     <t>Sequencing Core Tour (Optional)</t>
+  </si>
+  <si>
+    <t>Compute: Reproducible analysis (JG, KO)</t>
   </si>
 </sst>
 </file>
@@ -3989,7 +3989,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L15" sqref="L15"/>
       <selection pane="bottomLeft" activeCell="L15" sqref="L15"/>
-      <selection pane="bottomRight" activeCell="P1" sqref="P1:P1048576"/>
+      <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4616,7 +4616,7 @@
       </c>
       <c r="I21" s="133"/>
       <c r="J21" s="114" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="K21" s="133"/>
       <c r="L21" s="144" t="s">
@@ -4772,11 +4772,11 @@
       </c>
       <c r="I26" s="120"/>
       <c r="J26" s="109" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K26" s="120"/>
       <c r="L26" s="109" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M26" s="120"/>
       <c r="N26" s="111" t="s">
@@ -4790,7 +4790,7 @@
       </c>
       <c r="C27" s="133"/>
       <c r="D27" s="114" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E27" s="133"/>
       <c r="F27" s="114" t="s">
@@ -4802,11 +4802,11 @@
       </c>
       <c r="I27" s="133"/>
       <c r="J27" s="114" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K27" s="133"/>
       <c r="L27" s="109" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M27" s="133"/>
       <c r="N27" s="115" t="s">
@@ -4841,7 +4841,7 @@
         <v>43287</v>
       </c>
       <c r="D29" s="130" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E29" s="129">
         <f>E23+1</f>
@@ -4875,7 +4875,7 @@
       </c>
       <c r="C30" s="119"/>
       <c r="D30" s="109" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E30" s="119"/>
       <c r="F30" s="148" t="s">
@@ -4885,7 +4885,7 @@
       <c r="H30" s="86"/>
       <c r="I30" s="119"/>
       <c r="J30" s="157" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K30" s="119"/>
       <c r="L30" s="86"/>
@@ -5065,7 +5065,7 @@
         <v>96</v>
       </c>
       <c r="B47" s="92" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>